<commit_message>
Updated spreadsheet and Code comments
New updates to the spreadsheet:
-Support for Piecewise Non-Homogeneous cross sections
-Added various material properties
-Added specific weight
-Added orange color to cells that require updates when stringers are added
--(kept yellow for stringer centroid location)
Updates to the main MATLAB script
-Updated Title Block to reflect the change to GPL v3.0 license.
</commit_message>
<xml_diff>
--- a/src/Section Properties.xlsx
+++ b/src/Section Properties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\School\WSU\Semester 5\Flight Structures\FINAL PROJECT\Code and Spreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A174FBB-F986-459A-BE7A-DABE5011DC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AAF9D0-27AA-4C32-B089-8F3DB50719DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="-228" windowWidth="30720" windowHeight="16680" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="16680" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Section Properties" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Name of element</t>
   </si>
@@ -141,16 +141,88 @@
     <t>Ai(z'i-zbar)^2</t>
   </si>
   <si>
-    <t>Ai*(y'i-ybar)*(z'i-zbar)</t>
-  </si>
-  <si>
     <t>I~</t>
   </si>
   <si>
-    <t>=add data/update formula</t>
-  </si>
-  <si>
     <t>WARNING: DO NOT CHANGE THE LOCATION OF VALUES IN THIS SHEET, LOCATIONS ARE HARD CODED IN THE MATLAB CODE.</t>
+  </si>
+  <si>
+    <t>Ei (ksi)</t>
+  </si>
+  <si>
+    <t>Ei/ER</t>
+  </si>
+  <si>
+    <t>ER (ksi)</t>
+  </si>
+  <si>
+    <t>(Ei/ER)Ai</t>
+  </si>
+  <si>
+    <t>Ai(y'i-ybar)(z'i-zbar)</t>
+  </si>
+  <si>
+    <t>Ai*(y'i)</t>
+  </si>
+  <si>
+    <t>Ai*(z'i)</t>
+  </si>
+  <si>
+    <t>ybar*</t>
+  </si>
+  <si>
+    <t>zbar*</t>
+  </si>
+  <si>
+    <t>Iyy*</t>
+  </si>
+  <si>
+    <t>Izz*</t>
+  </si>
+  <si>
+    <t>Iyz*</t>
+  </si>
+  <si>
+    <t>I~*</t>
+  </si>
+  <si>
+    <t>y'i-ybar*</t>
+  </si>
+  <si>
+    <t>Ai(y'i-ybar*)^2</t>
+  </si>
+  <si>
+    <t>Ai(z'i-zbar*)^2</t>
+  </si>
+  <si>
+    <t>Ai(y'i-ybar*)(z'i-zbar*)</t>
+  </si>
+  <si>
+    <t>=add data</t>
+  </si>
+  <si>
+    <t>=update formula to add stringers in sum</t>
+  </si>
+  <si>
+    <t>z'i-zbar*</t>
+  </si>
+  <si>
+    <t>Ult Tens Strength (ksi)</t>
+  </si>
+  <si>
+    <t>Ult Comp Strength (ksi)</t>
+  </si>
+  <si>
+    <t>Poisson's ratio</t>
+  </si>
+  <si>
+    <t>Specific Weight (lbf/ft^3)</t>
+  </si>
+  <si>
+    <t>Not Avaliable</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
   </si>
 </sst>
 </file>
@@ -172,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +263,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -204,15 +282,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3812326-F393-4F18-B450-8E22F40B5680}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,9 +746,15 @@
     <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -714,10 +798,52 @@
         <v>34</v>
       </c>
       <c r="O1" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -756,11 +882,11 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>D2-$Q$3</f>
+        <f>D2-$AE$3</f>
         <v>0.56979635487546165</v>
       </c>
       <c r="L2">
-        <f>E2-$R$3</f>
+        <f>E2-$AF$3</f>
         <v>-0.31166592625587453</v>
       </c>
       <c r="M2">
@@ -775,26 +901,77 @@
         <f>C2*K2*L2</f>
         <v>-4.1621744231128535E-2</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="P2">
+        <v>255</v>
+      </c>
+      <c r="Q2">
+        <f>P2/$AE$7</f>
+        <v>0.1275</v>
+      </c>
+      <c r="R2">
+        <f>Q2*C2</f>
+        <v>2.9882812500000001E-2</v>
+      </c>
+      <c r="S2">
+        <f>R2*D2</f>
+        <v>9.3383789062500004E-4</v>
+      </c>
+      <c r="T2">
+        <f>R2*E2</f>
+        <v>-5.60302734375E-2</v>
+      </c>
+      <c r="U2">
+        <f>D2-$AE$5</f>
+        <v>0.55631911859611249</v>
+      </c>
+      <c r="V2">
+        <f>E2-$AF$5</f>
+        <v>-0.21897636946224064</v>
+      </c>
+      <c r="W2">
+        <f>C2*U2^2</f>
+        <v>7.253694415208331E-2</v>
+      </c>
+      <c r="X2">
+        <f>C2*V2^2</f>
+        <v>1.1238433683483684E-2</v>
+      </c>
+      <c r="Y2">
+        <f>C2*U2*V2</f>
+        <v>-2.8551736137330561E-2</v>
+      </c>
+      <c r="Z2">
+        <v>1.47</v>
+      </c>
+      <c r="AA2">
+        <v>3</v>
+      </c>
+      <c r="AB2">
+        <v>0.35</v>
+      </c>
+      <c r="AC2">
+        <v>5.6</v>
+      </c>
+      <c r="AE2" t="s">
         <v>30</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AF2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" t="s">
+      <c r="AG2" t="s">
         <v>5</v>
       </c>
-      <c r="T2" t="s">
+      <c r="AH2" t="s">
         <v>6</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AI2" t="s">
         <v>7</v>
       </c>
-      <c r="V2" t="s">
-        <v>36</v>
+      <c r="AJ2" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -833,11 +1010,11 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>D3-$Q$3</f>
+        <f>D3-$AE$3</f>
         <v>-0.46145364512453835</v>
       </c>
       <c r="L3">
-        <f>E3-$R$3</f>
+        <f>E3-$AF$3</f>
         <v>-0.31166592625587453</v>
       </c>
       <c r="M3">
@@ -852,32 +1029,83 @@
         <f t="shared" ref="O3:O15" si="4">C3*K3*L3</f>
         <v>3.4885580384644552E-2</v>
       </c>
+      <c r="P3">
+        <v>255</v>
+      </c>
       <c r="Q3">
+        <f>P3/$AE$7</f>
+        <v>0.1275</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R15" si="5">Q3*C3</f>
+        <v>3.0927066777705518E-2</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S15" si="6">R3*D3</f>
+        <v>-3.0927066777705518E-2</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T15" si="7">R3*E3</f>
+        <v>-5.7988250208197846E-2</v>
+      </c>
+      <c r="U3">
+        <f>D3-$AE$5</f>
+        <v>-0.47493088140388751</v>
+      </c>
+      <c r="V3">
+        <f>E3-$AF$5</f>
+        <v>-0.21897636946224064</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W15" si="8">C3*U3^2</f>
+        <v>5.4712853614152887E-2</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X15" si="9">C3*V3^2</f>
+        <v>1.163116052098225E-2</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y15" si="10">C3*U3*V3</f>
+        <v>2.5226454030386754E-2</v>
+      </c>
+      <c r="Z3">
+        <v>1.47</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>0.35</v>
+      </c>
+      <c r="AC3">
+        <v>5.6</v>
+      </c>
+      <c r="AE3">
         <f>F16/C16</f>
         <v>-0.53854635487546165</v>
       </c>
-      <c r="R3">
+      <c r="AF3">
         <f>G16/C16</f>
         <v>-1.5633340737441255</v>
       </c>
-      <c r="S3">
+      <c r="AG3">
         <f>H16+N16</f>
-        <v>1.3303343231691338</v>
-      </c>
-      <c r="T3">
+        <v>1.3301308726482999</v>
+      </c>
+      <c r="AH3">
         <f>I16+M16</f>
-        <v>0.16643134242473706</v>
-      </c>
-      <c r="U3">
+        <v>0.16622789190390372</v>
+      </c>
+      <c r="AI3">
         <f>J16+O16</f>
         <v>-0.10454809147352823</v>
       </c>
-      <c r="V3">
-        <f>(S3*T3)-U3^2</f>
-        <v>0.2104790238479857</v>
+      <c r="AJ3">
+        <f>(AG3*AH3)-AI3^2</f>
+        <v>0.21017454748586947</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -916,11 +1144,11 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>D4-$Q$3</f>
+        <f>D4-$AE$3</f>
         <v>-0.21145364512453835</v>
       </c>
       <c r="L4">
-        <f>E4-$R$3</f>
+        <f>E4-$AF$3</f>
         <v>1.5008340737441255</v>
       </c>
       <c r="M4">
@@ -935,8 +1163,77 @@
         <f t="shared" si="4"/>
         <v>-5.9504406678807284E-2</v>
       </c>
+      <c r="P4">
+        <v>155</v>
+      </c>
+      <c r="Q4">
+        <f>P4/$AE$7</f>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="5"/>
+        <v>1.4531249999999999E-2</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="6"/>
+        <v>-1.08984375E-2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="7"/>
+        <v>-9.0820312499999994E-4</v>
+      </c>
+      <c r="U4">
+        <f>D4-$AE$5</f>
+        <v>-0.22493088140388751</v>
+      </c>
+      <c r="V4">
+        <f>E4-$AF$5</f>
+        <v>1.5935236305377594</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="8"/>
+        <v>9.4863565142118203E-3</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="9"/>
+        <v>0.4761220427029203</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="10"/>
+        <v>-6.7206126516521442E-2</v>
+      </c>
+      <c r="Z4">
+        <v>0.63</v>
+      </c>
+      <c r="AA4">
+        <v>1.46</v>
+      </c>
+      <c r="AB4">
+        <v>0.35</v>
+      </c>
+      <c r="AC4">
+        <v>5.3</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -975,11 +1272,11 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>D5-$Q$3</f>
+        <f>D5-$AE$3</f>
         <v>0.28854635487546165</v>
       </c>
       <c r="L5">
-        <f>E5-$R$3</f>
+        <f>E5-$AF$3</f>
         <v>-2.1241659262558743</v>
       </c>
       <c r="M5">
@@ -994,8 +1291,83 @@
         <f t="shared" si="4"/>
         <v>-3.8307520948236952E-2</v>
       </c>
+      <c r="P5">
+        <v>155</v>
+      </c>
+      <c r="Q5">
+        <f>P5/$AE$7</f>
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="5"/>
+        <v>4.84375E-3</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="6"/>
+        <v>-1.2109375E-3</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="7"/>
+        <v>-1.7861328124999999E-2</v>
+      </c>
+      <c r="U5">
+        <f>D5-$AE$5</f>
+        <v>0.27506911859611249</v>
+      </c>
+      <c r="V5">
+        <f>E5-$AF$5</f>
+        <v>-2.0314763694622409</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="8"/>
+        <v>4.7289387503276379E-3</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="9"/>
+        <v>0.25793101498021792</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="10"/>
+        <v>-3.4924775899800573E-2</v>
+      </c>
+      <c r="Z5">
+        <v>0.63</v>
+      </c>
+      <c r="AA5">
+        <v>1.46</v>
+      </c>
+      <c r="AB5">
+        <v>0.35</v>
+      </c>
+      <c r="AC5">
+        <v>5.3</v>
+      </c>
+      <c r="AE5">
+        <f>S16/R16</f>
+        <v>-0.52506911859611249</v>
+      </c>
+      <c r="AF5">
+        <f>T16/R16</f>
+        <v>-1.6560236305377594</v>
+      </c>
+      <c r="AG5">
+        <f>H16+X16</f>
+        <v>1.3363762734532507</v>
+      </c>
+      <c r="AH5">
+        <f>I16+W16</f>
+        <v>0.16635993034510801</v>
+      </c>
+      <c r="AI5">
+        <f>J16+Y16</f>
+        <v>-0.10545618452326581</v>
+      </c>
+      <c r="AJ5">
+        <f>(AG5*AH5)-AI5^2</f>
+        <v>0.21119845691233272</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1033,11 +1405,11 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>D6-$Q$3</f>
+        <f>D6-$AE$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L6" t="e">
-        <f>E6-$R$3</f>
+        <f>E6-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M6">
@@ -1052,8 +1424,62 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P6">
+        <v>1130</v>
+      </c>
+      <c r="Q6">
+        <f>P6/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="6"/>
+        <v>1.1035156249999999E-3</v>
+      </c>
+      <c r="T6" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U6">
+        <f>D6-$AE$5</f>
+        <v>0.65006911859611249</v>
+      </c>
+      <c r="V6" t="e">
+        <f>E6-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="8"/>
+        <v>6.602966546130103E-3</v>
+      </c>
+      <c r="X6" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z6">
+        <v>7.8</v>
+      </c>
+      <c r="AA6">
+        <v>7.8</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1061,11 +1487,11 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C15" si="5">0.125*0.125</f>
+        <f t="shared" ref="C7:C15" si="11">0.125*0.125</f>
         <v>1.5625E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D10" si="6">(1/16)+(1/8)/2</f>
+        <f t="shared" ref="D7:D10" si="12">(1/16)+(1/8)/2</f>
         <v>0.125</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1080,22 +1506,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:I15" si="7">((1/8)^4)/12</f>
+        <f t="shared" ref="H7:I15" si="13">((1/8)^4)/12</f>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>D7-$Q$3</f>
+        <f>D7-$AE$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L7" t="e">
-        <f>E7-$R$3</f>
+        <f>E7-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M7">
@@ -1110,8 +1536,62 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P7">
+        <v>1130</v>
+      </c>
+      <c r="Q7">
+        <f>P7/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="6"/>
+        <v>1.1035156249999999E-3</v>
+      </c>
+      <c r="T7" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U7">
+        <f>D7-$AE$5</f>
+        <v>0.65006911859611249</v>
+      </c>
+      <c r="V7" t="e">
+        <f>E7-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="8"/>
+        <v>6.602966546130103E-3</v>
+      </c>
+      <c r="X7" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y7" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z7">
+        <v>7.8</v>
+      </c>
+      <c r="AA7">
+        <v>7.8</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE7">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1119,11 +1599,11 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.125</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1138,22 +1618,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <f>D8-$Q$3</f>
+        <f>D8-$AE$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L8" t="e">
-        <f>E8-$R$3</f>
+        <f>E8-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M8">
@@ -1168,8 +1648,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P8">
+        <v>1130</v>
+      </c>
+      <c r="Q8">
+        <f>P8/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="6"/>
+        <v>1.1035156249999999E-3</v>
+      </c>
+      <c r="T8" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U8">
+        <f>D8-$AE$5</f>
+        <v>0.65006911859611249</v>
+      </c>
+      <c r="V8" t="e">
+        <f>E8-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="8"/>
+        <v>6.602966546130103E-3</v>
+      </c>
+      <c r="X8" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y8" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z8">
+        <v>7.8</v>
+      </c>
+      <c r="AA8">
+        <v>7.8</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1177,11 +1708,11 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.125</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -1196,22 +1727,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <f>D9-$Q$3</f>
+        <f>D9-$AE$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L9" t="e">
-        <f>E9-$R$3</f>
+        <f>E9-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M9">
@@ -1226,8 +1757,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P9">
+        <v>1130</v>
+      </c>
+      <c r="Q9">
+        <f>P9/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="6"/>
+        <v>1.1035156249999999E-3</v>
+      </c>
+      <c r="T9" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U9">
+        <f>D9-$AE$5</f>
+        <v>0.65006911859611249</v>
+      </c>
+      <c r="V9" t="e">
+        <f>E9-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="8"/>
+        <v>6.602966546130103E-3</v>
+      </c>
+      <c r="X9" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y9" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9">
+        <v>7.8</v>
+      </c>
+      <c r="AA9">
+        <v>7.8</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1235,11 +1817,11 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.125</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -1254,22 +1836,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <f>D10-$Q$3</f>
+        <f>D10-$AE$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L10" t="e">
-        <f>E10-$R$3</f>
+        <f>E10-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M10">
@@ -1284,8 +1866,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P10">
+        <v>1130</v>
+      </c>
+      <c r="Q10">
+        <f>P10/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="6"/>
+        <v>1.1035156249999999E-3</v>
+      </c>
+      <c r="T10" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U10">
+        <f>D10-$AE$5</f>
+        <v>0.65006911859611249</v>
+      </c>
+      <c r="V10" t="e">
+        <f>E10-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="8"/>
+        <v>6.602966546130103E-3</v>
+      </c>
+      <c r="X10" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y10" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z10">
+        <v>7.8</v>
+      </c>
+      <c r="AA10">
+        <v>7.8</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1311,22 +1944,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="e">
-        <f>D11-$Q$3</f>
+        <f>D11-$AE$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L11" t="e">
-        <f>E11-$R$3</f>
+        <f>E11-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M11" t="e">
@@ -1341,8 +1974,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P11">
+        <v>1130</v>
+      </c>
+      <c r="Q11">
+        <f>P11/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S11" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T11" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U11" t="e">
+        <f>D11-$AE$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V11" t="e">
+        <f>E11-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W11" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X11" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z11">
+        <v>7.8</v>
+      </c>
+      <c r="AA11">
+        <v>7.8</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1350,7 +2034,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1368,22 +2052,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="e">
-        <f>D12-$Q$3</f>
+        <f>D12-$AE$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L12" t="e">
-        <f>E12-$R$3</f>
+        <f>E12-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M12" t="e">
@@ -1398,8 +2082,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P12">
+        <v>1130</v>
+      </c>
+      <c r="Q12">
+        <f>P12/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S12" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T12" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U12" t="e">
+        <f>D12-$AE$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V12" t="e">
+        <f>E12-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W12" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X12" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y12" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z12">
+        <v>7.8</v>
+      </c>
+      <c r="AA12">
+        <v>7.8</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1407,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1425,22 +2160,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="e">
-        <f>D13-$Q$3</f>
+        <f>D13-$AE$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L13" t="e">
-        <f>E13-$R$3</f>
+        <f>E13-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M13" t="e">
@@ -1455,8 +2190,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P13">
+        <v>1130</v>
+      </c>
+      <c r="Q13">
+        <f>P13/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S13" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T13" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U13" t="e">
+        <f>D13-$AE$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V13" t="e">
+        <f>E13-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W13" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X13" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y13" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z13">
+        <v>7.8</v>
+      </c>
+      <c r="AA13">
+        <v>7.8</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1464,7 +2250,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1482,22 +2268,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="e">
-        <f>D14-$Q$3</f>
+        <f>D14-$AE$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L14" t="e">
-        <f>E14-$R$3</f>
+        <f>E14-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M14" t="e">
@@ -1512,8 +2298,59 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P14">
+        <v>1130</v>
+      </c>
+      <c r="Q14">
+        <f>P14/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S14" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T14" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U14" t="e">
+        <f>D14-$AE$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V14" t="e">
+        <f>E14-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W14" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X14" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y14" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z14">
+        <v>7.8</v>
+      </c>
+      <c r="AA14">
+        <v>7.8</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1521,7 +2358,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1539,22 +2376,22 @@
         <v>#VALUE!</v>
       </c>
       <c r="H15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="e">
-        <f>D15-$Q$3</f>
+        <f>D15-$AE$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L15" t="e">
-        <f>E15-$R$3</f>
+        <f>E15-$AF$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M15" t="e">
@@ -1569,59 +2406,140 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
+      <c r="P15">
+        <v>1130</v>
+      </c>
+      <c r="Q15">
+        <f>P15/$AE$7</f>
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="5"/>
+        <v>8.8281249999999992E-3</v>
+      </c>
+      <c r="S15" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T15" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U15" t="e">
+        <f>D15-$AE$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V15" t="e">
+        <f>E15-$AF$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W15" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="X15" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Y15" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z15">
+        <v>7.8</v>
+      </c>
+      <c r="AA15">
+        <v>7.8</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <f>SUM(C2:C5)</f>
         <v>0.72694022962906291</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="3">
         <f>SUM(F2:F5)</f>
         <v>-0.39149101087906291</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
         <f>SUM(G2:G5)</f>
         <v>-1.1364504305544929</v>
       </c>
-      <c r="H16">
-        <f>SUM(H2:H15)</f>
-        <v>0.57965707208648032</v>
-      </c>
-      <c r="I16">
-        <f>SUM(I2:I15)</f>
-        <v>2.5098287835165697E-2</v>
-      </c>
-      <c r="J16">
-        <f>SUM(J2:J15)</f>
+      <c r="H16" s="3">
+        <f>SUM(H2:H5)</f>
+        <v>0.57945362156564661</v>
+      </c>
+      <c r="I16" s="3">
+        <f>SUM(I2:I5)</f>
+        <v>2.4894837314332376E-2</v>
+      </c>
+      <c r="J16" s="3">
+        <f>SUM(J2:J5)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="1">
+      <c r="M16" s="3">
         <f>SUM(M2:M5)</f>
         <v>0.14133305458957135</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="3">
         <f>SUM(N2:N5)</f>
         <v>0.75067725108265337</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="3">
         <f>SUM(O2:O5)</f>
         <v>-0.10454809147352823</v>
+      </c>
+      <c r="R16" s="3">
+        <f>SUM(R2:R5)</f>
+        <v>8.0184879277705512E-2</v>
+      </c>
+      <c r="S16" s="3">
+        <f>SUM(S2:S5)</f>
+        <v>-4.2102603887080516E-2</v>
+      </c>
+      <c r="T16" s="3">
+        <f>SUM(T2:T5)</f>
+        <v>-0.13278805489569784</v>
+      </c>
+      <c r="W16" s="3">
+        <f>SUM(W2:W5)</f>
+        <v>0.14146509303077565</v>
+      </c>
+      <c r="X16" s="3">
+        <f>SUM(X2:X5)</f>
+        <v>0.75692265188760421</v>
+      </c>
+      <c r="Y16" s="3">
+        <f>SUM(Y2:Y5)</f>
+        <v>-0.10545618452326581</v>
       </c>
     </row>
     <row r="21" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q21" s="1"/>
-      <c r="R21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
+      <c r="R21" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q22" s="3"/>
+      <c r="R22" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="23" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1646,9 +2564,8 @@
       <c r="V25" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="Q23:V25"/>
-    <mergeCell ref="R21:T21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Various Updates to Spreadsheet and MATLAB Code
Spreadsheet Changes:
-Added Volume (in^3), Rib x Location (in), and Boundary points for max distance from neutral axis calculations
StructuresCalc.m Changes:
-Removed code to retrieve data from spreadsheet to a function named datafromsheet.m
-changed function inputs in pseudocode from the previous long form to "alldata" the output from the new function datafromsheet.m
Created datafromsheet.m:
-created new function to handle retrieving the data
-outputs "alldata" a cell array of matrices
-"all data" now contains all relevant values from the spreadsheet
</commit_message>
<xml_diff>
--- a/src/Section Properties.xlsx
+++ b/src/Section Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AAF9D0-27AA-4C32-B089-8F3DB50719DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08D8A9C-AD60-4434-981F-D609545D70FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="16680" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
+    <workbookView xWindow="5616" yWindow="2868" windowWidth="30720" windowHeight="16680" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Section Properties" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>Name of element</t>
   </si>
@@ -223,6 +223,42 @@
   </si>
   <si>
     <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>Shear Modulus (ksi)</t>
+  </si>
+  <si>
+    <t>LE Top Skin y</t>
+  </si>
+  <si>
+    <t>TE Top Skin y</t>
+  </si>
+  <si>
+    <t>LE Bottom Skin y</t>
+  </si>
+  <si>
+    <t>TE Bottom Skin y</t>
+  </si>
+  <si>
+    <t>LE Top Skin z</t>
+  </si>
+  <si>
+    <t>LE Bottom Skin z</t>
+  </si>
+  <si>
+    <t>TE Top Skin z</t>
+  </si>
+  <si>
+    <t>TE Bottom Skin z</t>
+  </si>
+  <si>
+    <t>Volume (in^3)</t>
+  </si>
+  <si>
+    <t>Rib x Location (in)</t>
+  </si>
+  <si>
+    <t>^ need to subtract more than 1/16, which is an estimate</t>
   </si>
 </sst>
 </file>
@@ -285,12 +321,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,6 +448,66 @@
         <a:xfrm>
           <a:off x="5829300" y="3055621"/>
           <a:ext cx="5509260" cy="4126084"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="190500" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="70000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>457675</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>53695</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{172DF825-8A7B-44BE-93A0-9E653997D04B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26883360" y="3086100"/>
+          <a:ext cx="5486875" cy="4099915"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -730,10 +826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3812326-F393-4F18-B450-8E22F40B5680}">
-  <dimension ref="A1:AJ25"/>
+  <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,10 +847,16 @@
     <col min="25" max="26" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.77734375" customWidth="1"/>
+    <col min="30" max="30" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,10 +942,19 @@
         <v>59</v>
       </c>
       <c r="AC1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" t="s">
         <v>60</v>
       </c>
+      <c r="AE1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -882,11 +993,11 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>D2-$AE$3</f>
+        <f>D2-$AH$3</f>
         <v>0.56979635487546165</v>
       </c>
       <c r="L2">
-        <f>E2-$AF$3</f>
+        <f>E2-$AI$3</f>
         <v>-0.31166592625587453</v>
       </c>
       <c r="M2">
@@ -905,7 +1016,7 @@
         <v>255</v>
       </c>
       <c r="Q2">
-        <f>P2/$AE$7</f>
+        <f>P2/$AH$7</f>
         <v>0.1275</v>
       </c>
       <c r="R2">
@@ -921,11 +1032,11 @@
         <v>-5.60302734375E-2</v>
       </c>
       <c r="U2">
-        <f>D2-$AE$5</f>
+        <f>D2-$AH$5</f>
         <v>0.55631911859611249</v>
       </c>
       <c r="V2">
-        <f>E2-$AF$5</f>
+        <f>E2-$AI$5</f>
         <v>-0.21897636946224064</v>
       </c>
       <c r="W2">
@@ -950,28 +1061,37 @@
         <v>0.35</v>
       </c>
       <c r="AC2">
+        <v>36</v>
+      </c>
+      <c r="AD2">
         <v>5.6</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AI2" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AJ2" t="s">
         <v>5</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AK2" t="s">
         <v>6</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AL2" t="s">
         <v>7</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AM2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1010,11 +1130,11 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>D3-$AE$3</f>
+        <f>D3-$AH$3</f>
         <v>-0.46145364512453835</v>
       </c>
       <c r="L3">
-        <f>E3-$AF$3</f>
+        <f>E3-$AI$3</f>
         <v>-0.31166592625587453</v>
       </c>
       <c r="M3">
@@ -1033,7 +1153,7 @@
         <v>255</v>
       </c>
       <c r="Q3">
-        <f>P3/$AE$7</f>
+        <f>P3/$AH$7</f>
         <v>0.1275</v>
       </c>
       <c r="R3">
@@ -1049,11 +1169,11 @@
         <v>-5.7988250208197846E-2</v>
       </c>
       <c r="U3">
-        <f>D3-$AE$5</f>
+        <f>D3-$AH$5</f>
         <v>-0.47493088140388751</v>
       </c>
       <c r="V3">
-        <f>E3-$AF$5</f>
+        <f>E3-$AI$5</f>
         <v>-0.21897636946224064</v>
       </c>
       <c r="W3">
@@ -1078,34 +1198,43 @@
         <v>0.35</v>
       </c>
       <c r="AC3">
+        <v>36</v>
+      </c>
+      <c r="AD3">
         <v>5.6</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH3">
         <f>F16/C16</f>
         <v>-0.53854635487546165</v>
       </c>
-      <c r="AF3">
+      <c r="AI3">
         <f>G16/C16</f>
         <v>-1.5633340737441255</v>
       </c>
-      <c r="AG3">
+      <c r="AJ3">
         <f>H16+N16</f>
         <v>1.3301308726482999</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <f>I16+M16</f>
         <v>0.16622789190390372</v>
       </c>
-      <c r="AI3">
+      <c r="AL3">
         <f>J16+O16</f>
         <v>-0.10454809147352823</v>
       </c>
-      <c r="AJ3">
-        <f>(AG3*AH3)-AI3^2</f>
+      <c r="AM3">
+        <f>(AJ3*AK3)-AL3^2</f>
         <v>0.21017454748586947</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1144,11 +1273,11 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>D4-$AE$3</f>
+        <f>D4-$AH$3</f>
         <v>-0.21145364512453835</v>
       </c>
       <c r="L4">
-        <f>E4-$AF$3</f>
+        <f>E4-$AI$3</f>
         <v>1.5008340737441255</v>
       </c>
       <c r="M4">
@@ -1167,7 +1296,7 @@
         <v>155</v>
       </c>
       <c r="Q4">
-        <f>P4/$AE$7</f>
+        <f>P4/$AH$7</f>
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="R4">
@@ -1183,11 +1312,11 @@
         <v>-9.0820312499999994E-4</v>
       </c>
       <c r="U4">
-        <f>D4-$AE$5</f>
+        <f>D4-$AH$5</f>
         <v>-0.22493088140388751</v>
       </c>
       <c r="V4">
-        <f>E4-$AF$5</f>
+        <f>E4-$AI$5</f>
         <v>1.5935236305377594</v>
       </c>
       <c r="W4">
@@ -1212,28 +1341,37 @@
         <v>0.35</v>
       </c>
       <c r="AC4">
+        <v>36</v>
+      </c>
+      <c r="AD4">
         <v>5.3</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH4" t="s">
         <v>44</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AI4" t="s">
         <v>45</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AJ4" t="s">
         <v>46</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AK4" t="s">
         <v>47</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AL4" t="s">
         <v>48</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AM4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1272,11 +1410,11 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>D5-$AE$3</f>
+        <f>D5-$AH$3</f>
         <v>0.28854635487546165</v>
       </c>
       <c r="L5">
-        <f>E5-$AF$3</f>
+        <f>E5-$AI$3</f>
         <v>-2.1241659262558743</v>
       </c>
       <c r="M5">
@@ -1295,7 +1433,7 @@
         <v>155</v>
       </c>
       <c r="Q5">
-        <f>P5/$AE$7</f>
+        <f>P5/$AH$7</f>
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="R5">
@@ -1311,11 +1449,11 @@
         <v>-1.7861328124999999E-2</v>
       </c>
       <c r="U5">
-        <f>D5-$AE$5</f>
+        <f>D5-$AH$5</f>
         <v>0.27506911859611249</v>
       </c>
       <c r="V5">
-        <f>E5-$AF$5</f>
+        <f>E5-$AI$5</f>
         <v>-2.0314763694622409</v>
       </c>
       <c r="W5">
@@ -1340,34 +1478,43 @@
         <v>0.35</v>
       </c>
       <c r="AC5">
+        <v>36</v>
+      </c>
+      <c r="AD5">
         <v>5.3</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH5">
         <f>S16/R16</f>
         <v>-0.52506911859611249</v>
       </c>
-      <c r="AF5">
+      <c r="AI5">
         <f>T16/R16</f>
         <v>-1.6560236305377594</v>
       </c>
-      <c r="AG5">
+      <c r="AJ5">
         <f>H16+X16</f>
         <v>1.3363762734532507</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <f>I16+W16</f>
         <v>0.16635993034510801</v>
       </c>
-      <c r="AI5">
+      <c r="AL5">
         <f>J16+Y16</f>
         <v>-0.10545618452326581</v>
       </c>
-      <c r="AJ5">
-        <f>(AG5*AH5)-AI5^2</f>
+      <c r="AM5">
+        <f>(AJ5*AK5)-AL5^2</f>
         <v>0.21119845691233272</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1405,11 +1552,11 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>D6-$AE$3</f>
+        <f>D6-$AH$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L6" t="e">
-        <f>E6-$AF$3</f>
+        <f>E6-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M6">
@@ -1428,7 +1575,7 @@
         <v>1130</v>
       </c>
       <c r="Q6">
-        <f>P6/$AE$7</f>
+        <f>P6/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R6">
@@ -1444,11 +1591,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U6">
-        <f>D6-$AE$5</f>
+        <f>D6-$AH$5</f>
         <v>0.65006911859611249</v>
       </c>
       <c r="V6" t="e">
-        <f>E6-$AF$5</f>
+        <f>E6-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W6">
@@ -1472,14 +1619,23 @@
       <c r="AB6" t="s">
         <v>62</v>
       </c>
-      <c r="AC6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE6" t="s">
+      <c r="AC6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1517,11 +1673,11 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>D7-$AE$3</f>
+        <f>D7-$AH$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L7" t="e">
-        <f>E7-$AF$3</f>
+        <f>E7-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M7">
@@ -1540,7 +1696,7 @@
         <v>1130</v>
       </c>
       <c r="Q7">
-        <f>P7/$AE$7</f>
+        <f>P7/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R7">
@@ -1556,11 +1712,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U7">
-        <f>D7-$AE$5</f>
+        <f>D7-$AH$5</f>
         <v>0.65006911859611249</v>
       </c>
       <c r="V7" t="e">
-        <f>E7-$AF$5</f>
+        <f>E7-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W7">
@@ -1584,14 +1740,23 @@
       <c r="AB7" t="s">
         <v>62</v>
       </c>
-      <c r="AC7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE7">
+      <c r="AC7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH7">
         <v>2000</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1629,11 +1794,11 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <f>D8-$AE$3</f>
+        <f>D8-$AH$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L8" t="e">
-        <f>E8-$AF$3</f>
+        <f>E8-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M8">
@@ -1652,7 +1817,7 @@
         <v>1130</v>
       </c>
       <c r="Q8">
-        <f>P8/$AE$7</f>
+        <f>P8/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R8">
@@ -1668,11 +1833,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U8">
-        <f>D8-$AE$5</f>
+        <f>D8-$AH$5</f>
         <v>0.65006911859611249</v>
       </c>
       <c r="V8" t="e">
-        <f>E8-$AF$5</f>
+        <f>E8-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W8">
@@ -1696,11 +1861,20 @@
       <c r="AB8" t="s">
         <v>62</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AC8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1738,11 +1912,11 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <f>D9-$AE$3</f>
+        <f>D9-$AH$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L9" t="e">
-        <f>E9-$AF$3</f>
+        <f>E9-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M9">
@@ -1761,7 +1935,7 @@
         <v>1130</v>
       </c>
       <c r="Q9">
-        <f>P9/$AE$7</f>
+        <f>P9/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R9">
@@ -1777,11 +1951,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U9">
-        <f>D9-$AE$5</f>
+        <f>D9-$AH$5</f>
         <v>0.65006911859611249</v>
       </c>
       <c r="V9" t="e">
-        <f>E9-$AF$5</f>
+        <f>E9-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W9">
@@ -1805,11 +1979,32 @@
       <c r="AB9" t="s">
         <v>62</v>
       </c>
-      <c r="AC9" t="s">
-        <v>61</v>
+      <c r="AC9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1847,11 +2042,11 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <f>D10-$AE$3</f>
+        <f>D10-$AH$3</f>
         <v>0.66354635487546165</v>
       </c>
       <c r="L10" t="e">
-        <f>E10-$AF$3</f>
+        <f>E10-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M10">
@@ -1870,7 +2065,7 @@
         <v>1130</v>
       </c>
       <c r="Q10">
-        <f>P10/$AE$7</f>
+        <f>P10/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R10">
@@ -1886,11 +2081,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U10">
-        <f>D10-$AE$5</f>
+        <f>D10-$AH$5</f>
         <v>0.65006911859611249</v>
       </c>
       <c r="V10" t="e">
-        <f>E10-$AF$5</f>
+        <f>E10-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W10">
@@ -1914,11 +2109,34 @@
       <c r="AB10" t="s">
         <v>62</v>
       </c>
-      <c r="AC10" t="s">
-        <v>61</v>
+      <c r="AC10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH10">
+        <f>1/16</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="1">
+        <f>-1.5-(1/16)</f>
+        <v>-1.5625</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1955,11 +2173,11 @@
         <v>0</v>
       </c>
       <c r="K11" t="e">
-        <f>D11-$AE$3</f>
+        <f>D11-$AH$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L11" t="e">
-        <f>E11-$AF$3</f>
+        <f>E11-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M11" t="e">
@@ -1978,7 +2196,7 @@
         <v>1130</v>
       </c>
       <c r="Q11">
-        <f>P11/$AE$7</f>
+        <f>P11/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R11">
@@ -1994,11 +2212,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U11" t="e">
-        <f>D11-$AE$5</f>
+        <f>D11-$AH$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="V11" t="e">
-        <f>E11-$AF$5</f>
+        <f>E11-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W11" t="e">
@@ -2022,11 +2240,32 @@
       <c r="AB11" t="s">
         <v>62</v>
       </c>
-      <c r="AC11" t="s">
-        <v>61</v>
+      <c r="AC11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2063,11 +2302,11 @@
         <v>0</v>
       </c>
       <c r="K12" t="e">
-        <f>D12-$AE$3</f>
+        <f>D12-$AH$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L12" t="e">
-        <f>E12-$AF$3</f>
+        <f>E12-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M12" t="e">
@@ -2086,7 +2325,7 @@
         <v>1130</v>
       </c>
       <c r="Q12">
-        <f>P12/$AE$7</f>
+        <f>P12/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R12">
@@ -2102,11 +2341,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U12" t="e">
-        <f>D12-$AE$5</f>
+        <f>D12-$AH$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="V12" t="e">
-        <f>E12-$AF$5</f>
+        <f>E12-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W12" t="e">
@@ -2130,11 +2369,34 @@
       <c r="AB12" t="s">
         <v>62</v>
       </c>
-      <c r="AC12" t="s">
-        <v>61</v>
+      <c r="AC12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH12">
+        <f>1/16</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="AI12">
+        <v>-3.75</v>
+      </c>
+      <c r="AJ12" s="1">
+        <f>-0.5-(1/16)</f>
+        <v>-0.5625</v>
+      </c>
+      <c r="AK12">
+        <v>-3.75</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2171,11 +2433,11 @@
         <v>0</v>
       </c>
       <c r="K13" t="e">
-        <f>D13-$AE$3</f>
+        <f>D13-$AH$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L13" t="e">
-        <f>E13-$AF$3</f>
+        <f>E13-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M13" t="e">
@@ -2194,7 +2456,7 @@
         <v>1130</v>
       </c>
       <c r="Q13">
-        <f>P13/$AE$7</f>
+        <f>P13/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R13">
@@ -2210,11 +2472,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U13" t="e">
-        <f>D13-$AE$5</f>
+        <f>D13-$AH$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="V13" t="e">
-        <f>E13-$AF$5</f>
+        <f>E13-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W13" t="e">
@@ -2238,11 +2500,20 @@
       <c r="AB13" t="s">
         <v>62</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AC13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF13" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2279,11 +2550,11 @@
         <v>0</v>
       </c>
       <c r="K14" t="e">
-        <f>D14-$AE$3</f>
+        <f>D14-$AH$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L14" t="e">
-        <f>E14-$AF$3</f>
+        <f>E14-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M14" t="e">
@@ -2302,7 +2573,7 @@
         <v>1130</v>
       </c>
       <c r="Q14">
-        <f>P14/$AE$7</f>
+        <f>P14/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R14">
@@ -2318,11 +2589,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U14" t="e">
-        <f>D14-$AE$5</f>
+        <f>D14-$AH$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="V14" t="e">
-        <f>E14-$AF$5</f>
+        <f>E14-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W14" t="e">
@@ -2346,11 +2617,23 @@
       <c r="AB14" t="s">
         <v>62</v>
       </c>
-      <c r="AC14" t="s">
-        <v>61</v>
+      <c r="AC14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ14" t="s">
+        <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2387,11 +2670,11 @@
         <v>0</v>
       </c>
       <c r="K15" t="e">
-        <f>D15-$AE$3</f>
+        <f>D15-$AH$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="L15" t="e">
-        <f>E15-$AF$3</f>
+        <f>E15-$AI$3</f>
         <v>#VALUE!</v>
       </c>
       <c r="M15" t="e">
@@ -2410,7 +2693,7 @@
         <v>1130</v>
       </c>
       <c r="Q15">
-        <f>P15/$AE$7</f>
+        <f>P15/$AH$7</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="R15">
@@ -2426,11 +2709,11 @@
         <v>#VALUE!</v>
       </c>
       <c r="U15" t="e">
-        <f>D15-$AE$5</f>
+        <f>D15-$AH$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="V15" t="e">
-        <f>E15-$AF$5</f>
+        <f>E15-$AI$5</f>
         <v>#VALUE!</v>
       </c>
       <c r="W15" t="e">
@@ -2454,114 +2737,123 @@
       <c r="AB15" t="s">
         <v>62</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AC15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF15" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <f>SUM(C2:C5)</f>
         <v>0.72694022962906291</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <f>SUM(F2:F5)</f>
         <v>-0.39149101087906291</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <f>SUM(G2:G5)</f>
         <v>-1.1364504305544929</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <f>SUM(H2:H5)</f>
         <v>0.57945362156564661</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <f>SUM(I2:I5)</f>
         <v>2.4894837314332376E-2</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <f>SUM(J2:J5)</f>
         <v>0</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="2">
         <f>SUM(M2:M5)</f>
         <v>0.14133305458957135</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <f>SUM(N2:N5)</f>
         <v>0.75067725108265337</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="2">
         <f>SUM(O2:O5)</f>
         <v>-0.10454809147352823</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="2">
         <f>SUM(R2:R5)</f>
         <v>8.0184879277705512E-2</v>
       </c>
-      <c r="S16" s="3">
+      <c r="S16" s="2">
         <f>SUM(S2:S5)</f>
         <v>-4.2102603887080516E-2</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16" s="2">
         <f>SUM(T2:T5)</f>
         <v>-0.13278805489569784</v>
       </c>
-      <c r="W16" s="3">
+      <c r="W16" s="2">
         <f>SUM(W2:W5)</f>
         <v>0.14146509303077565</v>
       </c>
-      <c r="X16" s="3">
+      <c r="X16" s="2">
         <f>SUM(X2:X5)</f>
         <v>0.75692265188760421</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16" s="2">
         <f>SUM(Y2:Y5)</f>
         <v>-0.10545618452326581</v>
       </c>
     </row>
     <row r="21" spans="17:22" x14ac:dyDescent="0.3">
       <c r="Q21" s="1"/>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
     </row>
     <row r="22" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q22" s="3"/>
-      <c r="R22" s="4" t="s">
+      <c r="Q22" s="2"/>
+      <c r="R22" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q23" s="2" t="s">
+      <c r="Q23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="R23" s="2"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5"/>
+      <c r="V23" s="5"/>
     </row>
     <row r="24" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
     </row>
     <row r="25" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added Needed Values to Spreadsheet and updated datafromsheet.m
Changes to the spreadsheet:
- Added additional values according to issue #12 .
- Calculated areas of LE,TE spars and bottom skins as trapezoids (because they are not rectangles)
- Calculated new locations of centroids for the trapezoidal sections
- Correctly calculated the bottom Z positions of the bottom skin surface for the maximum stress calculation function, accounting for the trapezoidal shapes.
Changes to datafromsheet.m:
- Updated "alldata" creation to include new data values added to the spreadsheet.
</commit_message>
<xml_diff>
--- a/src/Section Properties.xlsx
+++ b/src/Section Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08D8A9C-AD60-4434-981F-D609545D70FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEFFBFA-4DA6-445F-AF40-8AFD2D30156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5616" yWindow="2868" windowWidth="30720" windowHeight="16680" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
+    <workbookView xWindow="13584" yWindow="1728" windowWidth="19464" windowHeight="11616" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Section Properties" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
   <si>
     <t>Name of element</t>
   </si>
@@ -258,7 +258,28 @@
     <t>Rib x Location (in)</t>
   </si>
   <si>
-    <t>^ need to subtract more than 1/16, which is an estimate</t>
+    <t>End Loads in the X Direction(lbf)</t>
+  </si>
+  <si>
+    <t>End Loads in the Y Direction(lbf)</t>
+  </si>
+  <si>
+    <t>Y Position along the Y-Axis(in)</t>
+  </si>
+  <si>
+    <t>Z Position along the Z-Axis(in)</t>
+  </si>
+  <si>
+    <t>End Loads in the Z Direction(lbf)</t>
+  </si>
+  <si>
+    <t>Length of the beam in X (in)</t>
+  </si>
+  <si>
+    <t>X position of End Loads (in)</t>
+  </si>
+  <si>
+    <t>P=100, Our Goal</t>
   </si>
 </sst>
 </file>
@@ -318,12 +339,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -826,11 +848,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3812326-F393-4F18-B450-8E22F40B5680}">
-  <dimension ref="A1:AM25"/>
+  <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AI16" sqref="AI16"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -854,9 +874,19 @@
     <col min="33" max="35" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="25" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -953,8 +983,38 @@
       <c r="AF1" t="s">
         <v>73</v>
       </c>
+      <c r="AO1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -993,30 +1053,30 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f>D2-$AH$3</f>
-        <v>0.56979635487546165</v>
+        <f t="shared" ref="K2:K15" si="0">D2-$AH$3</f>
+        <v>0.56591783718449529</v>
       </c>
       <c r="L2">
-        <f>E2-$AI$3</f>
-        <v>-0.31166592625587453</v>
+        <f t="shared" ref="L2:L15" si="1">E2-$AI$3</f>
+        <v>-0.3121279259654981</v>
       </c>
       <c r="M2">
         <f>C2*K2^2</f>
-        <v>7.6094035788131953E-2</v>
+        <v>7.5061640260213336E-2</v>
       </c>
       <c r="N2">
         <f>C2*L2^2</f>
-        <v>2.2766167872405988E-2</v>
+        <v>2.2833713008013311E-2</v>
       </c>
       <c r="O2">
         <f>C2*K2*L2</f>
-        <v>-4.1621744231128535E-2</v>
+        <v>-4.1399709559518036E-2</v>
       </c>
       <c r="P2">
         <v>255</v>
       </c>
       <c r="Q2">
-        <f>P2/$AH$7</f>
+        <f t="shared" ref="Q2:Q15" si="2">P2/$AH$7</f>
         <v>0.1275</v>
       </c>
       <c r="R2">
@@ -1032,24 +1092,24 @@
         <v>-5.60302734375E-2</v>
       </c>
       <c r="U2">
-        <f>D2-$AH$5</f>
-        <v>0.55631911859611249</v>
+        <f t="shared" ref="U2:U15" si="3">D2-$AH$5</f>
+        <v>0.5539642634627947</v>
       </c>
       <c r="V2">
-        <f>E2-$AI$5</f>
-        <v>-0.21897636946224064</v>
+        <f t="shared" ref="V2:V15" si="4">E2-$AI$5</f>
+        <v>-0.22084018128948202</v>
       </c>
       <c r="W2">
         <f>C2*U2^2</f>
-        <v>7.253694415208331E-2</v>
+        <v>7.1924157467314828E-2</v>
       </c>
       <c r="X2">
         <f>C2*V2^2</f>
-        <v>1.1238433683483684E-2</v>
+        <v>1.143055914186827E-2</v>
       </c>
       <c r="Y2">
         <f>C2*U2*V2</f>
-        <v>-2.8551736137330561E-2</v>
+        <v>-2.8672867586957335E-2</v>
       </c>
       <c r="Z2">
         <v>1.47</v>
@@ -1066,8 +1126,9 @@
       <c r="AD2">
         <v>5.6</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>29</v>
+      <c r="AE2" s="5">
+        <f>C2*$AX$2</f>
+        <v>10.78125</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>61</v>
@@ -1090,8 +1151,39 @@
       <c r="AM2" t="s">
         <v>35</v>
       </c>
+      <c r="AO2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR2">
+        <v>5</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <f>-AI3</f>
+        <v>1.5628720740345019</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX2">
+        <v>46</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1099,24 +1191,24 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>SQRT(1+3.75^2)*0.0625</f>
-        <v>0.24256522962906288</v>
+        <f>((2*SQRT(1+3.75^2)+(6/180))*0.0625)/2</f>
+        <v>0.24360689629572954</v>
       </c>
       <c r="D3">
         <f>SQRT(1+3.75^2)/2*SIN(ATAN(1/3.75))-1.5</f>
         <v>-1</v>
       </c>
       <c r="E3">
-        <f>-SQRT(1+3.75^2)/2*COS(ATAN(1/3.75))</f>
-        <v>-1.875</v>
+        <f>((-SQRT(1+3.75^2)+(3/180))/2)*COS(ATAN(1/3.75))</f>
+        <v>-1.8669480421699898</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="0">C3*D3</f>
-        <v>-0.24256522962906288</v>
+        <f t="shared" ref="F3:F15" si="5">C3*D3</f>
+        <v>-0.24360689629572954</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G15" si="1">C3*E3</f>
-        <v>-0.45480980555449291</v>
+        <f t="shared" ref="G3:G15" si="6">C3*E3</f>
+        <v>-0.45480141809842001</v>
       </c>
       <c r="H3">
         <f>((1/16)*(SQRT(1+3.75^2)^3))/12</f>
@@ -1130,63 +1222,63 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>D3-$AH$3</f>
-        <v>-0.46145364512453835</v>
+        <f t="shared" si="0"/>
+        <v>-0.46533216281550471</v>
       </c>
       <c r="L3">
-        <f>E3-$AI$3</f>
-        <v>-0.31166592625587453</v>
+        <f t="shared" si="1"/>
+        <v>-0.30407596813548787</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M15" si="2">C3*K3^2</f>
-        <v>5.1651710612609501E-2</v>
+        <f t="shared" ref="M3:M15" si="7">C3*K3^2</f>
+        <v>5.2749180981084789E-2</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N15" si="3">C3*L3^2</f>
-        <v>2.3561731147707529E-2</v>
+        <f t="shared" ref="N3:N15" si="8">C3*L3^2</f>
+        <v>2.252442820187571E-2</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O15" si="4">C3*K3*L3</f>
-        <v>3.4885580384644552E-2</v>
+        <f t="shared" ref="O3:O15" si="9">C3*K3*L3</f>
+        <v>3.4469481280056884E-2</v>
       </c>
       <c r="P3">
         <v>255</v>
       </c>
       <c r="Q3">
-        <f>P3/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.1275</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R15" si="5">Q3*C3</f>
-        <v>3.0927066777705518E-2</v>
+        <f t="shared" ref="R3:R15" si="10">Q3*C3</f>
+        <v>3.1059879277705517E-2</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S15" si="6">R3*D3</f>
-        <v>-3.0927066777705518E-2</v>
+        <f t="shared" ref="S3:S15" si="11">R3*D3</f>
+        <v>-3.1059879277705517E-2</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T15" si="7">R3*E3</f>
-        <v>-5.7988250208197846E-2</v>
+        <f t="shared" ref="T3:T15" si="12">R3*E3</f>
+        <v>-5.7987180807548548E-2</v>
       </c>
       <c r="U3">
-        <f>D3-$AH$5</f>
-        <v>-0.47493088140388751</v>
+        <f t="shared" si="3"/>
+        <v>-0.4772857365372053</v>
       </c>
       <c r="V3">
-        <f>E3-$AI$5</f>
-        <v>-0.21897636946224064</v>
+        <f t="shared" si="4"/>
+        <v>-0.21278822345947179</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W15" si="8">C3*U3^2</f>
-        <v>5.4712853614152887E-2</v>
+        <f t="shared" ref="W3:W15" si="13">C3*U3^2</f>
+        <v>5.5494058847647389E-2</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X15" si="9">C3*V3^2</f>
-        <v>1.163116052098225E-2</v>
+        <f t="shared" ref="X3:X15" si="14">C3*V3^2</f>
+        <v>1.1030234767472552E-2</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y15" si="10">C3*U3*V3</f>
-        <v>2.5226454030386754E-2</v>
+        <f t="shared" ref="Y3:Y15" si="15">C3*U3*V3</f>
+        <v>2.4740907365929168E-2</v>
       </c>
       <c r="Z3">
         <v>1.47</v>
@@ -1203,38 +1295,70 @@
       <c r="AD3">
         <v>5.6</v>
       </c>
-      <c r="AE3" s="1" t="s">
-        <v>29</v>
+      <c r="AE3" s="5">
+        <f t="shared" ref="AE3:AE15" si="16">C3*$AX$2</f>
+        <v>11.205917229603559</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH3">
         <f>F16/C16</f>
-        <v>-0.53854635487546165</v>
+        <v>-0.53466783718449529</v>
       </c>
       <c r="AI3">
         <f>G16/C16</f>
-        <v>-1.5633340737441255</v>
+        <v>-1.5628720740345019</v>
       </c>
       <c r="AJ3">
         <f>H16+N16</f>
-        <v>1.3301308726482999</v>
+        <v>1.3431179030816649</v>
       </c>
       <c r="AK3">
         <f>I16+M16</f>
-        <v>0.16622789190390372</v>
+        <v>0.16542169027461398</v>
       </c>
       <c r="AL3">
         <f>J16+O16</f>
-        <v>-0.10454809147352823</v>
+        <v>-0.10250059727701728</v>
       </c>
       <c r="AM3">
         <f>(AJ3*AK3)-AL3^2</f>
-        <v>0.21017454748586947</v>
+        <v>0.21167446132371889</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <f>-1.875-AI3</f>
+        <v>-0.3121279259654981</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1242,24 +1366,24 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f>1.5*0.125</f>
-        <v>0.1875</v>
+        <f>((3+(3/90))*0.125)/2</f>
+        <v>0.18958333333333333</v>
       </c>
       <c r="D4">
-        <f>-1.5/2</f>
-        <v>-0.75</v>
+        <f>(-1.5+(3/90))/2</f>
+        <v>-0.73333333333333328</v>
       </c>
       <c r="E4">
         <f>-1/16</f>
         <v>-6.25E-2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
-        <v>-0.140625</v>
+        <f t="shared" si="5"/>
+        <v>-0.13902777777777775</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
-        <v>-1.171875E-2</v>
+        <f t="shared" si="6"/>
+        <v>-1.1848958333333333E-2</v>
       </c>
       <c r="H4">
         <f>(1.5*(1/8)^3)/12</f>
@@ -1273,63 +1397,63 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>D4-$AH$3</f>
-        <v>-0.21145364512453835</v>
+        <f t="shared" si="0"/>
+        <v>-0.19866549614883799</v>
       </c>
       <c r="L4">
-        <f>E4-$AI$3</f>
-        <v>1.5008340737441255</v>
+        <f t="shared" si="1"/>
+        <v>1.5003720740345019</v>
       </c>
       <c r="M4">
-        <f t="shared" si="2"/>
-        <v>8.3836207568351619E-3</v>
+        <f t="shared" si="7"/>
+        <v>7.4824710870121268E-3</v>
       </c>
       <c r="N4">
-        <f t="shared" si="3"/>
-        <v>0.42234429692088504</v>
+        <f t="shared" si="8"/>
+        <v>0.42677414335286651</v>
       </c>
       <c r="O4">
-        <f t="shared" si="4"/>
-        <v>-5.9504406678807284E-2</v>
+        <f t="shared" si="9"/>
+        <v>-5.6509514139852522E-2</v>
       </c>
       <c r="P4">
         <v>155</v>
       </c>
       <c r="Q4">
-        <f>P4/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="R4">
-        <f t="shared" si="5"/>
-        <v>1.4531249999999999E-2</v>
+        <f t="shared" si="10"/>
+        <v>1.4692708333333332E-2</v>
       </c>
       <c r="S4">
-        <f t="shared" si="6"/>
-        <v>-1.08984375E-2</v>
+        <f t="shared" si="11"/>
+        <v>-1.0774652777777775E-2</v>
       </c>
       <c r="T4">
-        <f t="shared" si="7"/>
-        <v>-9.0820312499999994E-4</v>
+        <f t="shared" si="12"/>
+        <v>-9.1829427083333325E-4</v>
       </c>
       <c r="U4">
-        <f>D4-$AH$5</f>
-        <v>-0.22493088140388751</v>
+        <f t="shared" si="3"/>
+        <v>-0.21061906987053858</v>
       </c>
       <c r="V4">
-        <f>E4-$AI$5</f>
-        <v>1.5935236305377594</v>
+        <f t="shared" si="4"/>
+        <v>1.591659818710518</v>
       </c>
       <c r="W4">
-        <f t="shared" si="8"/>
-        <v>9.4863565142118203E-3</v>
+        <f t="shared" si="13"/>
+        <v>8.4099910957810501E-3</v>
       </c>
       <c r="X4">
-        <f t="shared" si="9"/>
-        <v>0.4761220427029203</v>
+        <f t="shared" si="14"/>
+        <v>0.48028681050683647</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="10"/>
-        <v>-6.7206126516521442E-2</v>
+        <f t="shared" si="15"/>
+        <v>-6.3554762211683033E-2</v>
       </c>
       <c r="Z4">
         <v>0.63</v>
@@ -1346,8 +1470,9 @@
       <c r="AD4">
         <v>5.3</v>
       </c>
-      <c r="AE4" s="1" t="s">
-        <v>29</v>
+      <c r="AE4" s="5">
+        <f t="shared" si="16"/>
+        <v>8.7208333333333332</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>61</v>
@@ -1370,8 +1495,39 @@
       <c r="AM4" t="s">
         <v>49</v>
       </c>
+      <c r="AO4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX4">
+        <f>AX2-0.375</f>
+        <v>45.625</v>
+      </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1379,8 +1535,8 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>0.5*0.125</f>
-        <v>6.25E-2</v>
+        <f>((1+(3/90))*0.125)/2</f>
+        <v>6.458333333333334E-2</v>
       </c>
       <c r="D5">
         <f>-0.5/2</f>
@@ -1391,12 +1547,12 @@
         <v>-3.6875</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>-1.5625E-2</v>
+        <f t="shared" si="5"/>
+        <v>-1.6145833333333335E-2</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>-0.23046875</v>
+        <f t="shared" si="6"/>
+        <v>-0.2381510416666667</v>
       </c>
       <c r="H5">
         <f>(0.5*(1/8)^3)/12</f>
@@ -1410,63 +1566,63 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>D5-$AH$3</f>
-        <v>0.28854635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.28466783718449529</v>
       </c>
       <c r="L5">
-        <f>E5-$AI$3</f>
-        <v>-2.1241659262558743</v>
+        <f t="shared" si="1"/>
+        <v>-2.1246279259654983</v>
       </c>
       <c r="M5">
-        <f t="shared" si="2"/>
-        <v>5.2036874319947406E-3</v>
+        <f t="shared" si="7"/>
+        <v>5.2335606319713502E-3</v>
       </c>
       <c r="N5">
-        <f t="shared" si="3"/>
-        <v>0.2820050551416548</v>
+        <f t="shared" si="8"/>
+        <v>0.29153199695326271</v>
       </c>
       <c r="O5">
-        <f t="shared" si="4"/>
-        <v>-3.8307520948236952E-2</v>
+        <f t="shared" si="9"/>
+        <v>-3.9060854857703609E-2</v>
       </c>
       <c r="P5">
         <v>155</v>
       </c>
       <c r="Q5">
-        <f>P5/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="R5">
-        <f t="shared" si="5"/>
-        <v>4.84375E-3</v>
+        <f t="shared" si="10"/>
+        <v>5.0052083333333337E-3</v>
       </c>
       <c r="S5">
-        <f t="shared" si="6"/>
-        <v>-1.2109375E-3</v>
+        <f t="shared" si="11"/>
+        <v>-1.2513020833333334E-3</v>
       </c>
       <c r="T5">
-        <f t="shared" si="7"/>
-        <v>-1.7861328124999999E-2</v>
+        <f t="shared" si="12"/>
+        <v>-1.8456705729166668E-2</v>
       </c>
       <c r="U5">
-        <f>D5-$AH$5</f>
-        <v>0.27506911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.2727142634627947</v>
       </c>
       <c r="V5">
-        <f>E5-$AI$5</f>
-        <v>-2.0314763694622409</v>
+        <f t="shared" si="4"/>
+        <v>-2.033340181289482</v>
       </c>
       <c r="W5">
-        <f t="shared" si="8"/>
-        <v>4.7289387503276379E-3</v>
+        <f t="shared" si="13"/>
+        <v>4.8032607382868598E-3</v>
       </c>
       <c r="X5">
-        <f t="shared" si="9"/>
-        <v>0.25793101498021792</v>
+        <f t="shared" si="14"/>
+        <v>0.26701800224632638</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="10"/>
-        <v>-3.4924775899800573E-2</v>
+        <f t="shared" si="15"/>
+        <v>-3.581280618166597E-2</v>
       </c>
       <c r="Z5">
         <v>0.63</v>
@@ -1483,38 +1639,66 @@
       <c r="AD5">
         <v>5.3</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>29</v>
+      <c r="AE5" s="5">
+        <f t="shared" si="16"/>
+        <v>2.9708333333333337</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH5">
         <f>S16/R16</f>
-        <v>-0.52506911859611249</v>
+        <v>-0.5227142634627947</v>
       </c>
       <c r="AI5">
         <f>T16/R16</f>
-        <v>-1.6560236305377594</v>
+        <v>-1.654159818710518</v>
       </c>
       <c r="AJ5">
         <f>H16+X16</f>
-        <v>1.3363762734532507</v>
+        <v>1.3492192282281503</v>
       </c>
       <c r="AK5">
         <f>I16+W16</f>
-        <v>0.16635993034510801</v>
+        <v>0.1655263054633625</v>
       </c>
       <c r="AL5">
         <f>J16+Y16</f>
-        <v>-0.10545618452326581</v>
+        <v>-0.10329952861437716</v>
       </c>
       <c r="AM5">
         <f>(AJ5*AK5)-AL5^2</f>
-        <v>0.21119845691233272</v>
+        <v>0.21266048149678249</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1533,11 +1717,11 @@
         <v>29</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="G6" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H6">
@@ -1552,62 +1736,62 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>D6-$AH$3</f>
-        <v>0.66354635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.65966783718449529</v>
       </c>
       <c r="L6" t="e">
-        <f>E6-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
-        <v>6.8795900791955014E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.79940086586984E-3</v>
       </c>
       <c r="N6" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O6" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P6">
         <v>1130</v>
       </c>
       <c r="Q6">
-        <f>P6/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1035156249999999E-3</v>
       </c>
       <c r="T6" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U6">
-        <f>D6-$AH$5</f>
-        <v>0.65006911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.6477142634627947</v>
       </c>
       <c r="V6" t="e">
-        <f>E6-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W6">
-        <f t="shared" si="8"/>
-        <v>6.602966546130103E-3</v>
+        <f t="shared" si="13"/>
+        <v>6.555215110830479E-3</v>
       </c>
       <c r="X6" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y6" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z6">
@@ -1625,8 +1809,9 @@
       <c r="AD6" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE6" s="1" t="s">
-        <v>29</v>
+      <c r="AE6" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF6" s="1" t="s">
         <v>61</v>
@@ -1634,8 +1819,35 @@
       <c r="AH6" t="s">
         <v>39</v>
       </c>
+      <c r="AO6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW6" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1643,92 +1855,92 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C15" si="11">0.125*0.125</f>
+        <f t="shared" ref="C7:C15" si="17">0.125*0.125</f>
         <v>1.5625E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D10" si="12">(1/16)+(1/8)/2</f>
+        <f t="shared" ref="D7:D10" si="18">(1/16)+(1/8)/2</f>
         <v>0.125</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="G7" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:I15" si="13">((1/8)^4)/12</f>
+        <f t="shared" ref="H7:I15" si="19">((1/8)^4)/12</f>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I7">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <f>D7-$AH$3</f>
-        <v>0.66354635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.65966783718449529</v>
       </c>
       <c r="L7" t="e">
-        <f>E7-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
-        <v>6.8795900791955014E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.79940086586984E-3</v>
       </c>
       <c r="N7" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O7" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P7">
         <v>1130</v>
       </c>
       <c r="Q7">
-        <f>P7/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1035156249999999E-3</v>
       </c>
       <c r="T7" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U7">
-        <f>D7-$AH$5</f>
-        <v>0.65006911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.6477142634627947</v>
       </c>
       <c r="V7" t="e">
-        <f>E7-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W7">
-        <f t="shared" si="8"/>
-        <v>6.602966546130103E-3</v>
+        <f t="shared" si="13"/>
+        <v>6.555215110830479E-3</v>
       </c>
       <c r="X7" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y7" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z7">
@@ -1746,8 +1958,9 @@
       <c r="AD7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE7" s="1" t="s">
-        <v>29</v>
+      <c r="AE7" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF7" s="1" t="s">
         <v>61</v>
@@ -1755,8 +1968,35 @@
       <c r="AH7">
         <v>2000</v>
       </c>
+      <c r="AO7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1764,92 +2004,92 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.125</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="G8" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I8">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <f>D8-$AH$3</f>
-        <v>0.66354635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.65966783718449529</v>
       </c>
       <c r="L8" t="e">
-        <f>E8-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
-        <v>6.8795900791955014E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.79940086586984E-3</v>
       </c>
       <c r="N8" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O8" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P8">
         <v>1130</v>
       </c>
       <c r="Q8">
-        <f>P8/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1035156249999999E-3</v>
       </c>
       <c r="T8" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U8">
-        <f>D8-$AH$5</f>
-        <v>0.65006911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.6477142634627947</v>
       </c>
       <c r="V8" t="e">
-        <f>E8-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W8">
-        <f t="shared" si="8"/>
-        <v>6.602966546130103E-3</v>
+        <f t="shared" si="13"/>
+        <v>6.555215110830479E-3</v>
       </c>
       <c r="X8" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y8" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z8">
@@ -1867,14 +2107,42 @@
       <c r="AD8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE8" s="1" t="s">
-        <v>29</v>
+      <c r="AE8" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF8" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="AO8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1882,92 +2150,92 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.125</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="G9" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <f>D9-$AH$3</f>
-        <v>0.66354635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.65966783718449529</v>
       </c>
       <c r="L9" t="e">
-        <f>E9-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M9">
-        <f t="shared" si="2"/>
-        <v>6.8795900791955014E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.79940086586984E-3</v>
       </c>
       <c r="N9" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O9" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P9">
         <v>1130</v>
       </c>
       <c r="Q9">
-        <f>P9/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1035156249999999E-3</v>
       </c>
       <c r="T9" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U9">
-        <f>D9-$AH$5</f>
-        <v>0.65006911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.6477142634627947</v>
       </c>
       <c r="V9" t="e">
-        <f>E9-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W9">
-        <f t="shared" si="8"/>
-        <v>6.602966546130103E-3</v>
+        <f t="shared" si="13"/>
+        <v>6.555215110830479E-3</v>
       </c>
       <c r="X9" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y9" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z9">
@@ -1985,8 +2253,9 @@
       <c r="AD9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE9" s="1" t="s">
-        <v>29</v>
+      <c r="AE9" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF9" s="1" t="s">
         <v>61</v>
@@ -2003,8 +2272,35 @@
       <c r="AK9" t="s">
         <v>69</v>
       </c>
+      <c r="AO9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2012,92 +2308,92 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0.125</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.953125E-3</v>
       </c>
       <c r="G10" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <f>D10-$AH$3</f>
-        <v>0.66354635487546165</v>
+        <f t="shared" si="0"/>
+        <v>0.65966783718449529</v>
       </c>
       <c r="L10" t="e">
-        <f>E10-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
-        <v>6.8795900791955014E-3</v>
+        <f t="shared" si="7"/>
+        <v>6.79940086586984E-3</v>
       </c>
       <c r="N10" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P10">
         <v>1130</v>
       </c>
       <c r="Q10">
-        <f>P10/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>1.1035156249999999E-3</v>
       </c>
       <c r="T10" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U10">
-        <f>D10-$AH$5</f>
-        <v>0.65006911859611249</v>
+        <f t="shared" si="3"/>
+        <v>0.6477142634627947</v>
       </c>
       <c r="V10" t="e">
-        <f>E10-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W10">
-        <f t="shared" si="8"/>
-        <v>6.602966546130103E-3</v>
+        <f t="shared" si="13"/>
+        <v>6.555215110830479E-3</v>
       </c>
       <c r="X10" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y10" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z10">
@@ -2115,8 +2411,9 @@
       <c r="AD10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE10" s="1" t="s">
-        <v>29</v>
+      <c r="AE10" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF10" s="1" t="s">
         <v>61</v>
@@ -2128,15 +2425,42 @@
       <c r="AI10">
         <v>0</v>
       </c>
-      <c r="AJ10" s="1">
-        <f>-1.5-(1/16)</f>
-        <v>-1.5625</v>
+      <c r="AJ10" s="5">
+        <f>-1.5-SQRT((1/16)^2+(3/180)^2)</f>
+        <v>-1.5646840612344168</v>
       </c>
       <c r="AK10">
         <v>0</v>
       </c>
+      <c r="AO10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV10" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2144,7 +2468,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -2154,81 +2478,81 @@
         <v>29</v>
       </c>
       <c r="F11" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G11" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11" t="e">
-        <f>D11-$AH$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="L11" t="e">
-        <f>E11-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M11" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N11" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O11" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P11">
         <v>1130</v>
       </c>
       <c r="Q11">
-        <f>P11/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S11" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="T11" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U11" t="e">
-        <f>D11-$AH$5</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="V11" t="e">
-        <f>E11-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W11" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
       <c r="X11" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y11" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z11">
@@ -2246,8 +2570,9 @@
       <c r="AD11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE11" s="1" t="s">
-        <v>29</v>
+      <c r="AE11" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF11" s="1" t="s">
         <v>61</v>
@@ -2264,8 +2589,35 @@
       <c r="AK11" t="s">
         <v>71</v>
       </c>
+      <c r="AO11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2273,7 +2625,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -2283,81 +2635,81 @@
         <v>29</v>
       </c>
       <c r="F12" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G12" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I12">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12" t="e">
-        <f>D12-$AH$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="L12" t="e">
-        <f>E12-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M12" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N12" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O12" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P12">
         <v>1130</v>
       </c>
       <c r="Q12">
-        <f>P12/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S12" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="T12" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U12" t="e">
-        <f>D12-$AH$5</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="V12" t="e">
-        <f>E12-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W12" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
       <c r="X12" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y12" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z12">
@@ -2375,8 +2727,9 @@
       <c r="AD12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE12" s="1" t="s">
-        <v>29</v>
+      <c r="AE12" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF12" s="1" t="s">
         <v>61</v>
@@ -2388,15 +2741,42 @@
       <c r="AI12">
         <v>-3.75</v>
       </c>
-      <c r="AJ12" s="1">
-        <f>-0.5-(1/16)</f>
-        <v>-0.5625</v>
+      <c r="AJ12" s="5">
+        <f>-0.5-SQRT((1/16)^2+(3/180)^2)</f>
+        <v>-0.56468406123441672</v>
       </c>
       <c r="AK12">
         <v>-3.75</v>
       </c>
+      <c r="AO12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2404,7 +2784,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2414,81 +2794,81 @@
         <v>29</v>
       </c>
       <c r="F13" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G13" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13" t="e">
-        <f>D13-$AH$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="L13" t="e">
-        <f>E13-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M13" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N13" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O13" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P13">
         <v>1130</v>
       </c>
       <c r="Q13">
-        <f>P13/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S13" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="T13" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U13" t="e">
-        <f>D13-$AH$5</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="V13" t="e">
-        <f>E13-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W13" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
       <c r="X13" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y13" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z13">
@@ -2506,14 +2886,42 @@
       <c r="AD13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE13" s="1" t="s">
-        <v>29</v>
+      <c r="AE13" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF13" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="AO13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV13" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW13" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2521,7 +2929,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2531,81 +2939,81 @@
         <v>29</v>
       </c>
       <c r="F14" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G14" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I14">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
       <c r="K14" t="e">
-        <f>D14-$AH$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="L14" t="e">
-        <f>E14-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M14" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N14" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O14" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P14">
         <v>1130</v>
       </c>
       <c r="Q14">
-        <f>P14/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S14" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="T14" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U14" t="e">
-        <f>D14-$AH$5</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="V14" t="e">
-        <f>E14-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W14" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
       <c r="X14" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y14" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z14">
@@ -2623,17 +3031,42 @@
       <c r="AD14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE14" s="1" t="s">
-        <v>29</v>
+      <c r="AE14" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AJ14" t="s">
-        <v>74</v>
+      <c r="AO14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW14" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2641,7 +3074,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1.5625E-2</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -2651,81 +3084,81 @@
         <v>29</v>
       </c>
       <c r="F15" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="G15" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
       <c r="H15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="I15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>2.0345052083333332E-5</v>
       </c>
       <c r="J15">
         <v>0</v>
       </c>
       <c r="K15" t="e">
-        <f>D15-$AH$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="L15" t="e">
-        <f>E15-$AI$3</f>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
       <c r="M15" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
       <c r="N15" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="O15" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
       <c r="P15">
         <v>1130</v>
       </c>
       <c r="Q15">
-        <f>P15/$AH$7</f>
+        <f t="shared" si="2"/>
         <v>0.56499999999999995</v>
       </c>
       <c r="R15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.8281249999999992E-3</v>
       </c>
       <c r="S15" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
       <c r="T15" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>#VALUE!</v>
       </c>
       <c r="U15" t="e">
-        <f>D15-$AH$5</f>
+        <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
       <c r="V15" t="e">
-        <f>E15-$AI$5</f>
+        <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
       <c r="W15" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
       <c r="X15" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y15" t="e">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z15">
@@ -2743,28 +3176,56 @@
       <c r="AD15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AE15" s="1" t="s">
-        <v>29</v>
+      <c r="AE15" s="5">
+        <f t="shared" si="16"/>
+        <v>0.71875</v>
       </c>
       <c r="AF15" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="AO15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW15" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2">
         <f>SUM(C2:C5)</f>
-        <v>0.72694022962906291</v>
+        <v>0.73214856296239617</v>
       </c>
       <c r="F16" s="2">
         <f>SUM(F2:F5)</f>
-        <v>-0.39149101087906291</v>
+        <v>-0.39145628865684062</v>
       </c>
       <c r="G16" s="2">
         <f>SUM(G2:G5)</f>
-        <v>-1.1364504305544929</v>
+        <v>-1.1442545430984201</v>
       </c>
       <c r="H16" s="2">
         <f>SUM(H2:H5)</f>
@@ -2780,39 +3241,39 @@
       </c>
       <c r="M16" s="2">
         <f>SUM(M2:M5)</f>
-        <v>0.14133305458957135</v>
+        <v>0.14052685296028161</v>
       </c>
       <c r="N16" s="2">
         <f>SUM(N2:N5)</f>
-        <v>0.75067725108265337</v>
+        <v>0.76366428151601817</v>
       </c>
       <c r="O16" s="2">
         <f>SUM(O2:O5)</f>
-        <v>-0.10454809147352823</v>
+        <v>-0.10250059727701728</v>
       </c>
       <c r="R16" s="2">
         <f>SUM(R2:R5)</f>
-        <v>8.0184879277705512E-2</v>
+        <v>8.064060844437218E-2</v>
       </c>
       <c r="S16" s="2">
         <f>SUM(S2:S5)</f>
-        <v>-4.2102603887080516E-2</v>
+        <v>-4.2151996248191631E-2</v>
       </c>
       <c r="T16" s="2">
         <f>SUM(T2:T5)</f>
-        <v>-0.13278805489569784</v>
+        <v>-0.13339245424504856</v>
       </c>
       <c r="W16" s="2">
         <f>SUM(W2:W5)</f>
-        <v>0.14146509303077565</v>
+        <v>0.14063146814903013</v>
       </c>
       <c r="X16" s="2">
         <f>SUM(X2:X5)</f>
-        <v>0.75692265188760421</v>
+        <v>0.7697656066625036</v>
       </c>
       <c r="Y16" s="2">
         <f>SUM(Y2:Y5)</f>
-        <v>-0.10545618452326581</v>
+        <v>-0.10329952861437716</v>
       </c>
     </row>
     <row r="21" spans="17:22" x14ac:dyDescent="0.3">
@@ -2830,30 +3291,30 @@
       </c>
     </row>
     <row r="23" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q23" s="5" t="s">
+      <c r="Q23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-      <c r="U23" s="5"/>
-      <c r="V23" s="5"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6"/>
     </row>
     <row r="24" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6"/>
     </row>
     <row r="25" spans="17:22" x14ac:dyDescent="0.3">
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Fixing conflicts in main for neurtral-axis branch
Fixing conflicts in main
</commit_message>
<xml_diff>
--- a/src/Section Properties.xlsx
+++ b/src/Section Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMAC_PC\Documents\GitHub\structures-calc\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEFFBFA-4DA6-445F-AF40-8AFD2D30156D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A3B8C9-5D73-46EB-8F19-C3312B698126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13584" yWindow="1728" windowWidth="19464" windowHeight="11616" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
+    <workbookView xWindow="0" yWindow="2292" windowWidth="30720" windowHeight="12828" xr2:uid="{F60304DA-B739-4F41-9D99-FD3530222EDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cross Section Properties" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="83">
   <si>
     <t>Name of element</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>P=100, Our Goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Below values are assumed to be in the blue axis (auxillary axes) coord system below:</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -348,6 +351,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -850,7 +856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3812326-F393-4F18-B450-8E22F40B5680}">
   <dimension ref="A1:AX25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AJ7" sqref="AJ7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1054,23 +1062,23 @@
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K15" si="0">D2-$AH$3</f>
-        <v>0.56591783718449529</v>
+        <v>0.56979635487546165</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L15" si="1">E2-$AI$3</f>
-        <v>-0.3121279259654981</v>
+        <v>-0.31166592625587453</v>
       </c>
       <c r="M2">
         <f>C2*K2^2</f>
-        <v>7.5061640260213336E-2</v>
+        <v>7.6094035788131953E-2</v>
       </c>
       <c r="N2">
         <f>C2*L2^2</f>
-        <v>2.2833713008013311E-2</v>
+        <v>2.2766167872405988E-2</v>
       </c>
       <c r="O2">
         <f>C2*K2*L2</f>
-        <v>-4.1399709559518036E-2</v>
+        <v>-4.1621744231128535E-2</v>
       </c>
       <c r="P2">
         <v>255</v>
@@ -1093,23 +1101,23 @@
       </c>
       <c r="U2">
         <f t="shared" ref="U2:U15" si="3">D2-$AH$5</f>
-        <v>0.5539642634627947</v>
+        <v>0.55631911859611249</v>
       </c>
       <c r="V2">
         <f t="shared" ref="V2:V15" si="4">E2-$AI$5</f>
-        <v>-0.22084018128948202</v>
+        <v>-0.21897636946224064</v>
       </c>
       <c r="W2">
         <f>C2*U2^2</f>
-        <v>7.1924157467314828E-2</v>
+        <v>7.253694415208331E-2</v>
       </c>
       <c r="X2">
         <f>C2*V2^2</f>
-        <v>1.143055914186827E-2</v>
+        <v>1.1238433683483684E-2</v>
       </c>
       <c r="Y2">
         <f>C2*U2*V2</f>
-        <v>-2.8672867586957335E-2</v>
+        <v>-2.8551736137330561E-2</v>
       </c>
       <c r="Z2">
         <v>1.47</v>
@@ -1168,7 +1176,7 @@
       </c>
       <c r="AT2">
         <f>-AI3</f>
-        <v>1.5628720740345019</v>
+        <v>1.5633340737441255</v>
       </c>
       <c r="AU2" t="s">
         <v>62</v>
@@ -1191,55 +1199,56 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>((2*SQRT(1+3.75^2)+(6/180))*0.0625)/2</f>
-        <v>0.24360689629572954</v>
+        <f>SQRT(1+3.75^2)*0.0625</f>
+        <v>0.24256522962906288</v>
       </c>
       <c r="D3">
         <f>SQRT(1+3.75^2)/2*SIN(ATAN(1/3.75))-1.5</f>
         <v>-1</v>
       </c>
       <c r="E3">
-        <f>((-SQRT(1+3.75^2)+(3/180))/2)*COS(ATAN(1/3.75))</f>
-        <v>-1.8669480421699898</v>
+        <f>(-SQRT(1+3.75^2)/2)*COS(ATAN(1/3.75))</f>
+        <v>-1.875</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F15" si="5">C3*D3</f>
-        <v>-0.24360689629572954</v>
+        <v>-0.24256522962906288</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G15" si="6">C3*E3</f>
-        <v>-0.45480141809842001</v>
+        <v>-0.45480980555449291</v>
       </c>
       <c r="H3">
-        <f>((1/16)*(SQRT(1+3.75^2)^3))/12</f>
-        <v>0.3044698976073133</v>
+        <f>(((1/16)*(SQRT(1+3.75^2)))/24)*((1/16)^2+(SQRT(1+3.75^2))^2)+(((1/16)*(SQRT(1+3.75^2)))/24)*((1/16)^2-(SQRT(1+3.75^2))^2)*COS(2*ATAN(1/3.75))</f>
+        <v>2.028748701139621E-2</v>
       </c>
       <c r="I3">
-        <f>(SQRT(1+3.75^2)*(1/16)^3)/12</f>
-        <v>7.8960035686543906E-5</v>
+        <f>(((1/16)*(SQRT(1+3.75^2)))/24)*((1/16)^2+(SQRT(1+3.75^2))^2)-(((1/16)*(SQRT(1+3.75^2)))/24)*((1/16)^2-(SQRT(1+3.75^2))^2)*COS(2*ATAN(1/3.75))</f>
+        <v>0.28426137063160367</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <f>(((1/16)*(SQRT(1+3.75^2)))/24)*((1/16)^2-(SQRT(1+3.75^2))^2)*SIN(2*ATAN(1/3.75))</f>
+        <v>-7.5781976158911218E-2</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>-0.46533216281550471</v>
+        <v>-0.46145364512453835</v>
       </c>
       <c r="L3">
         <f t="shared" si="1"/>
-        <v>-0.30407596813548787</v>
+        <v>-0.31166592625587453</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M15" si="7">C3*K3^2</f>
-        <v>5.2749180981084789E-2</v>
+        <v>5.1651710612609501E-2</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:N15" si="8">C3*L3^2</f>
-        <v>2.252442820187571E-2</v>
+        <v>2.3561731147707529E-2</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O15" si="9">C3*K3*L3</f>
-        <v>3.4469481280056884E-2</v>
+        <v>3.4885580384644552E-2</v>
       </c>
       <c r="P3">
         <v>255</v>
@@ -1250,35 +1259,35 @@
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R15" si="10">Q3*C3</f>
-        <v>3.1059879277705517E-2</v>
+        <v>3.0927066777705518E-2</v>
       </c>
       <c r="S3">
         <f t="shared" ref="S3:S15" si="11">R3*D3</f>
-        <v>-3.1059879277705517E-2</v>
+        <v>-3.0927066777705518E-2</v>
       </c>
       <c r="T3">
         <f t="shared" ref="T3:T15" si="12">R3*E3</f>
-        <v>-5.7987180807548548E-2</v>
+        <v>-5.7988250208197846E-2</v>
       </c>
       <c r="U3">
         <f t="shared" si="3"/>
-        <v>-0.4772857365372053</v>
+        <v>-0.47493088140388751</v>
       </c>
       <c r="V3">
         <f t="shared" si="4"/>
-        <v>-0.21278822345947179</v>
+        <v>-0.21897636946224064</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W15" si="13">C3*U3^2</f>
-        <v>5.5494058847647389E-2</v>
+        <v>5.4712853614152887E-2</v>
       </c>
       <c r="X3">
         <f t="shared" ref="X3:X15" si="14">C3*V3^2</f>
-        <v>1.1030234767472552E-2</v>
+        <v>1.163116052098225E-2</v>
       </c>
       <c r="Y3">
         <f t="shared" ref="Y3:Y15" si="15">C3*U3*V3</f>
-        <v>2.4740907365929168E-2</v>
+        <v>2.5226454030386754E-2</v>
       </c>
       <c r="Z3">
         <v>1.47</v>
@@ -1297,34 +1306,34 @@
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE15" si="16">C3*$AX$2</f>
-        <v>11.205917229603559</v>
+        <v>11.158000562936893</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH3">
         <f>F16/C16</f>
-        <v>-0.53466783718449529</v>
+        <v>-0.53854635487546165</v>
       </c>
       <c r="AI3">
         <f>G16/C16</f>
-        <v>-1.5628720740345019</v>
+        <v>-1.5633340737441255</v>
       </c>
       <c r="AJ3">
         <f>H16+N16</f>
-        <v>1.3431179030816649</v>
+        <v>1.0459484620523829</v>
       </c>
       <c r="AK3">
         <f>I16+M16</f>
-        <v>0.16542169027461398</v>
+        <v>0.45041030249982084</v>
       </c>
       <c r="AL3">
         <f>J16+O16</f>
-        <v>-0.10250059727701728</v>
+        <v>-0.18033006763243944</v>
       </c>
       <c r="AM3">
         <f>(AJ3*AK3)-AL3^2</f>
-        <v>0.21167446132371889</v>
+        <v>0.43858702989991594</v>
       </c>
       <c r="AO3" t="s">
         <v>62</v>
@@ -1343,7 +1352,7 @@
       </c>
       <c r="AT3">
         <f>-1.875-AI3</f>
-        <v>-0.3121279259654981</v>
+        <v>-0.31166592625587453</v>
       </c>
       <c r="AU3" t="s">
         <v>62</v>
@@ -1366,12 +1375,12 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f>((3+(3/90))*0.125)/2</f>
-        <v>0.18958333333333333</v>
+        <f>1.5*0.125</f>
+        <v>0.1875</v>
       </c>
       <c r="D4">
-        <f>(-1.5+(3/90))/2</f>
-        <v>-0.73333333333333328</v>
+        <f>(-1.5)/2</f>
+        <v>-0.75</v>
       </c>
       <c r="E4">
         <f>-1/16</f>
@@ -1379,11 +1388,11 @@
       </c>
       <c r="F4">
         <f t="shared" si="5"/>
-        <v>-0.13902777777777775</v>
+        <v>-0.140625</v>
       </c>
       <c r="G4">
         <f t="shared" si="6"/>
-        <v>-1.1848958333333333E-2</v>
+        <v>-1.171875E-2</v>
       </c>
       <c r="H4">
         <f>(1.5*(1/8)^3)/12</f>
@@ -1398,23 +1407,23 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>-0.19866549614883799</v>
+        <v>-0.21145364512453835</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>1.5003720740345019</v>
+        <v>1.5008340737441255</v>
       </c>
       <c r="M4">
         <f t="shared" si="7"/>
-        <v>7.4824710870121268E-3</v>
+        <v>8.3836207568351619E-3</v>
       </c>
       <c r="N4">
         <f t="shared" si="8"/>
-        <v>0.42677414335286651</v>
+        <v>0.42234429692088504</v>
       </c>
       <c r="O4">
         <f t="shared" si="9"/>
-        <v>-5.6509514139852522E-2</v>
+        <v>-5.9504406678807284E-2</v>
       </c>
       <c r="P4">
         <v>155</v>
@@ -1425,35 +1434,35 @@
       </c>
       <c r="R4">
         <f t="shared" si="10"/>
-        <v>1.4692708333333332E-2</v>
+        <v>1.4531249999999999E-2</v>
       </c>
       <c r="S4">
         <f t="shared" si="11"/>
-        <v>-1.0774652777777775E-2</v>
+        <v>-1.08984375E-2</v>
       </c>
       <c r="T4">
         <f t="shared" si="12"/>
-        <v>-9.1829427083333325E-4</v>
+        <v>-9.0820312499999994E-4</v>
       </c>
       <c r="U4">
         <f t="shared" si="3"/>
-        <v>-0.21061906987053858</v>
+        <v>-0.22493088140388751</v>
       </c>
       <c r="V4">
         <f t="shared" si="4"/>
-        <v>1.591659818710518</v>
+        <v>1.5935236305377594</v>
       </c>
       <c r="W4">
         <f t="shared" si="13"/>
-        <v>8.4099910957810501E-3</v>
+        <v>9.4863565142118203E-3</v>
       </c>
       <c r="X4">
         <f t="shared" si="14"/>
-        <v>0.48028681050683647</v>
+        <v>0.4761220427029203</v>
       </c>
       <c r="Y4">
         <f t="shared" si="15"/>
-        <v>-6.3554762211683033E-2</v>
+        <v>-6.7206126516521442E-2</v>
       </c>
       <c r="Z4">
         <v>0.63</v>
@@ -1472,7 +1481,7 @@
       </c>
       <c r="AE4" s="5">
         <f t="shared" si="16"/>
-        <v>8.7208333333333332</v>
+        <v>8.625</v>
       </c>
       <c r="AF4" s="1" t="s">
         <v>61</v>
@@ -1535,8 +1544,8 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>((1+(3/90))*0.125)/2</f>
-        <v>6.458333333333334E-2</v>
+        <f>0.5*0.125</f>
+        <v>6.25E-2</v>
       </c>
       <c r="D5">
         <f>-0.5/2</f>
@@ -1548,11 +1557,11 @@
       </c>
       <c r="F5">
         <f t="shared" si="5"/>
-        <v>-1.6145833333333335E-2</v>
+        <v>-1.5625E-2</v>
       </c>
       <c r="G5">
         <f t="shared" si="6"/>
-        <v>-0.2381510416666667</v>
+        <v>-0.23046875</v>
       </c>
       <c r="H5">
         <f>(0.5*(1/8)^3)/12</f>
@@ -1567,23 +1576,23 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0.28466783718449529</v>
+        <v>0.28854635487546165</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>-2.1246279259654983</v>
+        <v>-2.1241659262558743</v>
       </c>
       <c r="M5">
         <f t="shared" si="7"/>
-        <v>5.2335606319713502E-3</v>
+        <v>5.2036874319947406E-3</v>
       </c>
       <c r="N5">
         <f t="shared" si="8"/>
-        <v>0.29153199695326271</v>
+        <v>0.2820050551416548</v>
       </c>
       <c r="O5">
         <f t="shared" si="9"/>
-        <v>-3.9060854857703609E-2</v>
+        <v>-3.8307520948236952E-2</v>
       </c>
       <c r="P5">
         <v>155</v>
@@ -1594,35 +1603,35 @@
       </c>
       <c r="R5">
         <f t="shared" si="10"/>
-        <v>5.0052083333333337E-3</v>
+        <v>4.84375E-3</v>
       </c>
       <c r="S5">
         <f t="shared" si="11"/>
-        <v>-1.2513020833333334E-3</v>
+        <v>-1.2109375E-3</v>
       </c>
       <c r="T5">
         <f t="shared" si="12"/>
-        <v>-1.8456705729166668E-2</v>
+        <v>-1.7861328124999999E-2</v>
       </c>
       <c r="U5">
         <f t="shared" si="3"/>
-        <v>0.2727142634627947</v>
+        <v>0.27506911859611249</v>
       </c>
       <c r="V5">
         <f t="shared" si="4"/>
-        <v>-2.033340181289482</v>
+        <v>-2.0314763694622409</v>
       </c>
       <c r="W5">
         <f t="shared" si="13"/>
-        <v>4.8032607382868598E-3</v>
+        <v>4.7289387503276379E-3</v>
       </c>
       <c r="X5">
         <f t="shared" si="14"/>
-        <v>0.26701800224632638</v>
+        <v>0.25793101498021792</v>
       </c>
       <c r="Y5">
         <f t="shared" si="15"/>
-        <v>-3.581280618166597E-2</v>
+        <v>-3.4924775899800573E-2</v>
       </c>
       <c r="Z5">
         <v>0.63</v>
@@ -1641,34 +1650,34 @@
       </c>
       <c r="AE5" s="5">
         <f t="shared" si="16"/>
-        <v>2.9708333333333337</v>
+        <v>2.875</v>
       </c>
       <c r="AF5" s="1" t="s">
         <v>61</v>
       </c>
       <c r="AH5">
         <f>S16/R16</f>
-        <v>-0.5227142634627947</v>
+        <v>-0.52506911859611249</v>
       </c>
       <c r="AI5">
         <f>T16/R16</f>
-        <v>-1.654159818710518</v>
+        <v>-1.6560236305377594</v>
       </c>
       <c r="AJ5">
         <f>H16+X16</f>
-        <v>1.3492192282281503</v>
+        <v>1.0521938628573337</v>
       </c>
       <c r="AK5">
         <f>I16+W16</f>
-        <v>0.1655263054633625</v>
+        <v>0.45054234094102513</v>
       </c>
       <c r="AL5">
         <f>J16+Y16</f>
-        <v>-0.10329952861437716</v>
+        <v>-0.18123816068217702</v>
       </c>
       <c r="AM5">
         <f>(AJ5*AK5)-AL5^2</f>
-        <v>0.21266048149678249</v>
+        <v>0.44121061520806448</v>
       </c>
       <c r="AO5" t="s">
         <v>62</v>
@@ -1737,7 +1746,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0.65966783718449529</v>
+        <v>0.66354635487546165</v>
       </c>
       <c r="L6" t="e">
         <f t="shared" si="1"/>
@@ -1745,7 +1754,7 @@
       </c>
       <c r="M6">
         <f t="shared" si="7"/>
-        <v>6.79940086586984E-3</v>
+        <v>6.8795900791955014E-3</v>
       </c>
       <c r="N6" t="e">
         <f t="shared" si="8"/>
@@ -1776,7 +1785,7 @@
       </c>
       <c r="U6">
         <f t="shared" si="3"/>
-        <v>0.6477142634627947</v>
+        <v>0.65006911859611249</v>
       </c>
       <c r="V6" t="e">
         <f t="shared" si="4"/>
@@ -1784,7 +1793,7 @@
       </c>
       <c r="W6">
         <f t="shared" si="13"/>
-        <v>6.555215110830479E-3</v>
+        <v>6.602966546130103E-3</v>
       </c>
       <c r="X6" t="e">
         <f t="shared" si="14"/>
@@ -1886,7 +1895,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0.65966783718449529</v>
+        <v>0.66354635487546165</v>
       </c>
       <c r="L7" t="e">
         <f t="shared" si="1"/>
@@ -1894,7 +1903,7 @@
       </c>
       <c r="M7">
         <f t="shared" si="7"/>
-        <v>6.79940086586984E-3</v>
+        <v>6.8795900791955014E-3</v>
       </c>
       <c r="N7" t="e">
         <f t="shared" si="8"/>
@@ -1925,7 +1934,7 @@
       </c>
       <c r="U7">
         <f t="shared" si="3"/>
-        <v>0.6477142634627947</v>
+        <v>0.65006911859611249</v>
       </c>
       <c r="V7" t="e">
         <f t="shared" si="4"/>
@@ -1933,7 +1942,7 @@
       </c>
       <c r="W7">
         <f t="shared" si="13"/>
-        <v>6.555215110830479E-3</v>
+        <v>6.602966546130103E-3</v>
       </c>
       <c r="X7" t="e">
         <f t="shared" si="14"/>
@@ -2035,7 +2044,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0.65966783718449529</v>
+        <v>0.66354635487546165</v>
       </c>
       <c r="L8" t="e">
         <f t="shared" si="1"/>
@@ -2043,7 +2052,7 @@
       </c>
       <c r="M8">
         <f t="shared" si="7"/>
-        <v>6.79940086586984E-3</v>
+        <v>6.8795900791955014E-3</v>
       </c>
       <c r="N8" t="e">
         <f t="shared" si="8"/>
@@ -2074,7 +2083,7 @@
       </c>
       <c r="U8">
         <f t="shared" si="3"/>
-        <v>0.6477142634627947</v>
+        <v>0.65006911859611249</v>
       </c>
       <c r="V8" t="e">
         <f t="shared" si="4"/>
@@ -2082,7 +2091,7 @@
       </c>
       <c r="W8">
         <f t="shared" si="13"/>
-        <v>6.555215110830479E-3</v>
+        <v>6.602966546130103E-3</v>
       </c>
       <c r="X8" t="e">
         <f t="shared" si="14"/>
@@ -2114,6 +2123,14 @@
       <c r="AF8" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="AG8" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
       <c r="AO8" t="s">
         <v>62</v>
       </c>
@@ -2181,7 +2198,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>0.65966783718449529</v>
+        <v>0.66354635487546165</v>
       </c>
       <c r="L9" t="e">
         <f t="shared" si="1"/>
@@ -2189,7 +2206,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="7"/>
-        <v>6.79940086586984E-3</v>
+        <v>6.8795900791955014E-3</v>
       </c>
       <c r="N9" t="e">
         <f t="shared" si="8"/>
@@ -2220,7 +2237,7 @@
       </c>
       <c r="U9">
         <f t="shared" si="3"/>
-        <v>0.6477142634627947</v>
+        <v>0.65006911859611249</v>
       </c>
       <c r="V9" t="e">
         <f t="shared" si="4"/>
@@ -2228,7 +2245,7 @@
       </c>
       <c r="W9">
         <f t="shared" si="13"/>
-        <v>6.555215110830479E-3</v>
+        <v>6.602966546130103E-3</v>
       </c>
       <c r="X9" t="e">
         <f t="shared" si="14"/>
@@ -2339,7 +2356,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>0.65966783718449529</v>
+        <v>0.66354635487546165</v>
       </c>
       <c r="L10" t="e">
         <f t="shared" si="1"/>
@@ -2347,7 +2364,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
-        <v>6.79940086586984E-3</v>
+        <v>6.8795900791955014E-3</v>
       </c>
       <c r="N10" t="e">
         <f t="shared" si="8"/>
@@ -2378,7 +2395,7 @@
       </c>
       <c r="U10">
         <f t="shared" si="3"/>
-        <v>0.6477142634627947</v>
+        <v>0.65006911859611249</v>
       </c>
       <c r="V10" t="e">
         <f t="shared" si="4"/>
@@ -2386,7 +2403,7 @@
       </c>
       <c r="W10">
         <f t="shared" si="13"/>
-        <v>6.555215110830479E-3</v>
+        <v>6.602966546130103E-3</v>
       </c>
       <c r="X10" t="e">
         <f t="shared" si="14"/>
@@ -3217,63 +3234,63 @@
       </c>
       <c r="C16" s="2">
         <f>SUM(C2:C5)</f>
-        <v>0.73214856296239617</v>
+        <v>0.72694022962906291</v>
       </c>
       <c r="F16" s="2">
         <f>SUM(F2:F5)</f>
-        <v>-0.39145628865684062</v>
+        <v>-0.39149101087906291</v>
       </c>
       <c r="G16" s="2">
         <f>SUM(G2:G5)</f>
-        <v>-1.1442545430984201</v>
+        <v>-1.1364504305544929</v>
       </c>
       <c r="H16" s="2">
         <f>SUM(H2:H5)</f>
-        <v>0.57945362156564661</v>
+        <v>0.29527121096972953</v>
       </c>
       <c r="I16" s="2">
         <f>SUM(I2:I5)</f>
-        <v>2.4894837314332376E-2</v>
+        <v>0.30907724791024949</v>
       </c>
       <c r="J16" s="2">
         <f>SUM(J2:J5)</f>
-        <v>0</v>
+        <v>-7.5781976158911218E-2</v>
       </c>
       <c r="M16" s="2">
         <f>SUM(M2:M5)</f>
-        <v>0.14052685296028161</v>
+        <v>0.14133305458957135</v>
       </c>
       <c r="N16" s="2">
         <f>SUM(N2:N5)</f>
-        <v>0.76366428151601817</v>
+        <v>0.75067725108265337</v>
       </c>
       <c r="O16" s="2">
         <f>SUM(O2:O5)</f>
-        <v>-0.10250059727701728</v>
+        <v>-0.10454809147352823</v>
       </c>
       <c r="R16" s="2">
         <f>SUM(R2:R5)</f>
-        <v>8.064060844437218E-2</v>
+        <v>8.0184879277705512E-2</v>
       </c>
       <c r="S16" s="2">
         <f>SUM(S2:S5)</f>
-        <v>-4.2151996248191631E-2</v>
+        <v>-4.2102603887080516E-2</v>
       </c>
       <c r="T16" s="2">
         <f>SUM(T2:T5)</f>
-        <v>-0.13339245424504856</v>
+        <v>-0.13278805489569784</v>
       </c>
       <c r="W16" s="2">
         <f>SUM(W2:W5)</f>
-        <v>0.14063146814903013</v>
+        <v>0.14146509303077565</v>
       </c>
       <c r="X16" s="2">
         <f>SUM(X2:X5)</f>
-        <v>0.7697656066625036</v>
+        <v>0.75692265188760421</v>
       </c>
       <c r="Y16" s="2">
         <f>SUM(Y2:Y5)</f>
-        <v>-0.10329952861437716</v>
+        <v>-0.10545618452326581</v>
       </c>
     </row>
     <row r="21" spans="17:22" x14ac:dyDescent="0.3">
@@ -3317,8 +3334,9 @@
       <c r="V25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="Q23:V25"/>
+    <mergeCell ref="AG8:AL8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>